<commit_message>
begin update from jupyter to py
</commit_message>
<xml_diff>
--- a/data/reorder.xlsx
+++ b/data/reorder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
   <si>
     <t>Part Number</t>
   </si>
@@ -82,15 +82,15 @@
     <t>CR-S</t>
   </si>
   <si>
+    <t>EC-PS</t>
+  </si>
+  <si>
     <t>EX-MD-WH</t>
   </si>
   <si>
     <t>EX-SPH-AM</t>
   </si>
   <si>
-    <t>EX-WR</t>
-  </si>
-  <si>
     <t>EX-WW</t>
   </si>
   <si>
@@ -112,6 +112,9 @@
     <t>EXCH-C-WH</t>
   </si>
   <si>
+    <t>GR-EC-SC</t>
+  </si>
+  <si>
     <t>GRX-3000-15D-300</t>
   </si>
   <si>
@@ -127,9 +130,15 @@
     <t>LC-3CH-DP</t>
   </si>
   <si>
+    <t>LDR24-4A</t>
+  </si>
+  <si>
     <t>LDR8-40</t>
   </si>
   <si>
+    <t>LDR8-40-277 - Old Do Not USe</t>
+  </si>
+  <si>
     <t>LDR8-80</t>
   </si>
   <si>
@@ -166,6 +175,9 @@
     <t>T24/1200-230</t>
   </si>
   <si>
+    <t>T24/1200-277</t>
+  </si>
+  <si>
     <t>T24/150-230</t>
   </si>
   <si>
@@ -221,6 +233,21 @@
   </si>
   <si>
     <t>WFL-108</t>
+  </si>
+  <si>
+    <t>XMS-PS-6CH-NP</t>
+  </si>
+  <si>
+    <t>XTRI-100-RGB-Mtr</t>
+  </si>
+  <si>
+    <t>XTRI-150-RGB-Mtr</t>
+  </si>
+  <si>
+    <t>xTRI-300-RGB-Mtr</t>
+  </si>
+  <si>
+    <t>XTRI-50-RGB-Mtr</t>
   </si>
 </sst>
 </file>
@@ -606,7 +633,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z58"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -774,7 +801,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>4574</v>
+        <v>4514</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -789,10 +816,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>4574</v>
+        <v>4514</v>
       </c>
       <c r="H5" s="2">
-        <v>4574</v>
+        <v>4514</v>
       </c>
       <c r="I5" s="2">
         <v>5000</v>
@@ -815,10 +842,10 @@
         <v>4440</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -827,10 +854,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>4440</v>
+        <v>3928</v>
       </c>
       <c r="H6" s="2">
-        <v>4440</v>
+        <v>3928</v>
       </c>
       <c r="I6" s="2">
         <v>5000</v>
@@ -850,13 +877,13 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>30498</v>
+        <v>30043</v>
       </c>
       <c r="C7" s="2">
-        <v>3077</v>
+        <v>2730</v>
       </c>
       <c r="D7" s="2">
-        <v>2066</v>
+        <v>1719</v>
       </c>
       <c r="E7" s="2">
         <v>1011</v>
@@ -865,10 +892,10 @@
         <v>22000</v>
       </c>
       <c r="G7" s="2">
-        <v>49421</v>
+        <v>49313</v>
       </c>
       <c r="H7" s="2">
-        <v>48410</v>
+        <v>50324</v>
       </c>
       <c r="I7" s="2">
         <v>50000</v>
@@ -1040,7 +1067,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2">
-        <v>4229</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -1055,13 +1082,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>4229</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2">
-        <v>4229</v>
+        <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
@@ -1078,13 +1105,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>856</v>
+        <v>4229</v>
       </c>
       <c r="C13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
@@ -1093,13 +1120,13 @@
         <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>855</v>
+        <v>4229</v>
       </c>
       <c r="H13" s="2">
-        <v>855</v>
+        <v>4229</v>
       </c>
       <c r="I13" s="2">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="J13" s="3">
         <v>0</v>
@@ -1116,13 +1143,13 @@
         <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>856</v>
       </c>
       <c r="C14" s="2">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
@@ -1131,13 +1158,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>-300</v>
+        <v>855</v>
       </c>
       <c r="H14" s="2">
-        <v>-300</v>
+        <v>855</v>
       </c>
       <c r="I14" s="2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J14" s="3">
         <v>0</v>
@@ -1154,13 +1181,13 @@
         <v>25</v>
       </c>
       <c r="B15" s="2">
-        <v>4718</v>
+        <v>4696</v>
       </c>
       <c r="C15" s="2">
-        <v>900</v>
+        <v>878</v>
       </c>
       <c r="D15" s="2">
-        <v>900</v>
+        <v>878</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -1420,7 +1447,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="2">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2">
         <v>0</v>
@@ -1435,13 +1462,13 @@
         <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
-        <v>150</v>
+        <v>1000</v>
       </c>
       <c r="J22" s="3">
         <v>0</v>
@@ -1458,7 +1485,7 @@
         <v>33</v>
       </c>
       <c r="B23" s="2">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
@@ -1473,13 +1500,13 @@
         <v>0</v>
       </c>
       <c r="G23" s="2">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="H23" s="2">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="I23" s="2">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="J23" s="3">
         <v>0</v>
@@ -1496,7 +1523,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="2">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
@@ -1511,13 +1538,13 @@
         <v>0</v>
       </c>
       <c r="G24" s="2">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="H24" s="2">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="I24" s="2">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="J24" s="3">
         <v>0</v>
@@ -1534,7 +1561,7 @@
         <v>35</v>
       </c>
       <c r="B25" s="2">
-        <v>430</v>
+        <v>7</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -1549,13 +1576,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="2">
-        <v>430</v>
+        <v>7</v>
       </c>
       <c r="H25" s="2">
-        <v>430</v>
+        <v>7</v>
       </c>
       <c r="I25" s="2">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="J25" s="3">
         <v>0</v>
@@ -1572,7 +1599,7 @@
         <v>36</v>
       </c>
       <c r="B26" s="2">
-        <v>21</v>
+        <v>430</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
@@ -1587,13 +1614,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <v>21</v>
+        <v>430</v>
       </c>
       <c r="H26" s="2">
-        <v>21</v>
+        <v>430</v>
       </c>
       <c r="I26" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="J26" s="3">
         <v>0</v>
@@ -1610,13 +1637,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="2">
-        <v>1231</v>
+        <v>21</v>
       </c>
       <c r="C27" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
@@ -1625,13 +1652,13 @@
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <v>1211</v>
+        <v>21</v>
       </c>
       <c r="H27" s="2">
-        <v>1211</v>
+        <v>21</v>
       </c>
       <c r="I27" s="2">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="J27" s="3">
         <v>0</v>
@@ -1648,28 +1675,28 @@
         <v>38</v>
       </c>
       <c r="B28" s="2">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="C28" s="2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>504</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>640</v>
+        <v>0</v>
       </c>
       <c r="H28" s="2">
-        <v>640</v>
+        <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>1500</v>
+        <v>125</v>
       </c>
       <c r="J28" s="3">
         <v>0</v>
@@ -1686,13 +1713,13 @@
         <v>39</v>
       </c>
       <c r="B29" s="2">
-        <v>1419</v>
+        <v>1231</v>
       </c>
       <c r="C29" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E29" s="2">
         <v>0</v>
@@ -1701,10 +1728,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="2">
-        <v>1419</v>
+        <v>1211</v>
       </c>
       <c r="H29" s="2">
-        <v>1419</v>
+        <v>1211</v>
       </c>
       <c r="I29" s="2">
         <v>1500</v>
@@ -1745,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="2">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="J30" s="3">
         <v>0</v>
@@ -1762,28 +1789,28 @@
         <v>41</v>
       </c>
       <c r="B31" s="2">
-        <v>3673</v>
+        <v>157</v>
       </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D31" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <v>504</v>
       </c>
       <c r="G31" s="2">
-        <v>3673</v>
+        <v>640</v>
       </c>
       <c r="H31" s="2">
-        <v>3673</v>
+        <v>640</v>
       </c>
       <c r="I31" s="2">
-        <v>5000</v>
+        <v>1500</v>
       </c>
       <c r="J31" s="3">
         <v>0</v>
@@ -1800,7 +1827,7 @@
         <v>42</v>
       </c>
       <c r="B32" s="2">
-        <v>2507</v>
+        <v>1419</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -1815,13 +1842,13 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <v>2507</v>
+        <v>1419</v>
       </c>
       <c r="H32" s="2">
-        <v>2507</v>
+        <v>1419</v>
       </c>
       <c r="I32" s="2">
-        <v>5000</v>
+        <v>1500</v>
       </c>
       <c r="J32" s="3">
         <v>0</v>
@@ -1838,7 +1865,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -1853,13 +1880,13 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H33" s="2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="I33" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="J33" s="3">
         <v>0</v>
@@ -1876,7 +1903,7 @@
         <v>44</v>
       </c>
       <c r="B34" s="2">
-        <v>28</v>
+        <v>3673</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
@@ -1891,13 +1918,13 @@
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <v>28</v>
+        <v>3673</v>
       </c>
       <c r="H34" s="2">
-        <v>28</v>
+        <v>3673</v>
       </c>
       <c r="I34" s="2">
-        <v>30</v>
+        <v>5000</v>
       </c>
       <c r="J34" s="3">
         <v>0</v>
@@ -1914,7 +1941,7 @@
         <v>45</v>
       </c>
       <c r="B35" s="2">
-        <v>24</v>
+        <v>2507</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
@@ -1929,13 +1956,13 @@
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <v>24</v>
+        <v>2507</v>
       </c>
       <c r="H35" s="2">
-        <v>24</v>
+        <v>2507</v>
       </c>
       <c r="I35" s="2">
-        <v>25</v>
+        <v>5000</v>
       </c>
       <c r="J35" s="3">
         <v>0</v>
@@ -1952,13 +1979,13 @@
         <v>46</v>
       </c>
       <c r="B36" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C36" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D36" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
@@ -1967,13 +1994,13 @@
         <v>0</v>
       </c>
       <c r="G36" s="2">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H36" s="2">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="I36" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J36" s="3">
         <v>0</v>
@@ -1990,7 +2017,7 @@
         <v>47</v>
       </c>
       <c r="B37" s="2">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="C37" s="2">
         <v>0</v>
@@ -2005,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="G37" s="2">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="H37" s="2">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="I37" s="2">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="J37" s="3">
         <v>0</v>
@@ -2028,7 +2055,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="2">
-        <v>8451</v>
+        <v>24</v>
       </c>
       <c r="C38" s="2">
         <v>0</v>
@@ -2043,13 +2070,13 @@
         <v>0</v>
       </c>
       <c r="G38" s="2">
-        <v>8451</v>
+        <v>24</v>
       </c>
       <c r="H38" s="2">
-        <v>8451</v>
+        <v>24</v>
       </c>
       <c r="I38" s="2">
-        <v>10000</v>
+        <v>25</v>
       </c>
       <c r="J38" s="3">
         <v>0</v>
@@ -2066,13 +2093,13 @@
         <v>49</v>
       </c>
       <c r="B39" s="2">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C39" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D39" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E39" s="2">
         <v>0</v>
@@ -2081,13 +2108,13 @@
         <v>0</v>
       </c>
       <c r="G39" s="2">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H39" s="2">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I39" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J39" s="3">
         <v>0</v>
@@ -2104,7 +2131,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="2">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
@@ -2119,13 +2146,13 @@
         <v>0</v>
       </c>
       <c r="G40" s="2">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="H40" s="2">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="I40" s="2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="J40" s="3">
         <v>0</v>
@@ -2142,7 +2169,7 @@
         <v>51</v>
       </c>
       <c r="B41" s="2">
-        <v>17</v>
+        <v>8451</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
@@ -2157,13 +2184,13 @@
         <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>17</v>
+        <v>8451</v>
       </c>
       <c r="H41" s="2">
-        <v>17</v>
+        <v>8451</v>
       </c>
       <c r="I41" s="2">
-        <v>20</v>
+        <v>10000</v>
       </c>
       <c r="J41" s="3">
         <v>0</v>
@@ -2180,7 +2207,7 @@
         <v>52</v>
       </c>
       <c r="B42" s="2">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C42" s="2">
         <v>0</v>
@@ -2195,10 +2222,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="2">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H42" s="2">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I42" s="2">
         <v>20</v>
@@ -2218,7 +2245,7 @@
         <v>53</v>
       </c>
       <c r="B43" s="2">
-        <v>12507</v>
+        <v>0</v>
       </c>
       <c r="C43" s="2">
         <v>0</v>
@@ -2233,13 +2260,13 @@
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <v>12507</v>
+        <v>0</v>
       </c>
       <c r="H43" s="2">
-        <v>12507</v>
+        <v>0</v>
       </c>
       <c r="I43" s="2">
-        <v>15000</v>
+        <v>100</v>
       </c>
       <c r="J43" s="3">
         <v>0</v>
@@ -2256,7 +2283,7 @@
         <v>54</v>
       </c>
       <c r="B44" s="2">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C44" s="2">
         <v>0</v>
@@ -2271,13 +2298,13 @@
         <v>0</v>
       </c>
       <c r="G44" s="2">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H44" s="2">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="I44" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J44" s="3">
         <v>0</v>
@@ -2294,7 +2321,7 @@
         <v>55</v>
       </c>
       <c r="B45" s="2">
-        <v>13801</v>
+        <v>17</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
@@ -2309,13 +2336,13 @@
         <v>0</v>
       </c>
       <c r="G45" s="2">
-        <v>13801</v>
+        <v>17</v>
       </c>
       <c r="H45" s="2">
-        <v>13801</v>
+        <v>17</v>
       </c>
       <c r="I45" s="2">
-        <v>15000</v>
+        <v>20</v>
       </c>
       <c r="J45" s="3">
         <v>0</v>
@@ -2332,31 +2359,31 @@
         <v>56</v>
       </c>
       <c r="B46" s="2">
-        <v>277</v>
+        <v>9</v>
       </c>
       <c r="C46" s="2">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="E46" s="2">
         <v>0</v>
       </c>
       <c r="F46" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G46" s="2">
-        <v>247</v>
+        <v>9</v>
       </c>
       <c r="H46" s="2">
-        <v>247</v>
+        <v>9</v>
       </c>
       <c r="I46" s="2">
-        <v>250</v>
+        <v>20</v>
       </c>
       <c r="J46" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K46" s="3">
         <v>0</v>
@@ -2370,7 +2397,7 @@
         <v>57</v>
       </c>
       <c r="B47" s="2">
-        <v>29</v>
+        <v>12507</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -2385,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="G47" s="2">
-        <v>29</v>
+        <v>12507</v>
       </c>
       <c r="H47" s="2">
-        <v>29</v>
+        <v>12507</v>
       </c>
       <c r="I47" s="2">
-        <v>50</v>
+        <v>15000</v>
       </c>
       <c r="J47" s="3">
         <v>0</v>
@@ -2408,13 +2435,13 @@
         <v>58</v>
       </c>
       <c r="B48" s="2">
-        <v>273</v>
+        <v>2</v>
       </c>
       <c r="C48" s="2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D48" s="2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E48" s="2">
         <v>0</v>
@@ -2423,13 +2450,13 @@
         <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>249</v>
+        <v>2</v>
       </c>
       <c r="H48" s="2">
-        <v>249</v>
+        <v>2</v>
       </c>
       <c r="I48" s="2">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="J48" s="3">
         <v>0</v>
@@ -2446,7 +2473,7 @@
         <v>59</v>
       </c>
       <c r="B49" s="2">
-        <v>246</v>
+        <v>13801</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
@@ -2461,13 +2488,13 @@
         <v>0</v>
       </c>
       <c r="G49" s="2">
-        <v>246</v>
+        <v>13801</v>
       </c>
       <c r="H49" s="2">
-        <v>246</v>
+        <v>13801</v>
       </c>
       <c r="I49" s="2">
-        <v>250</v>
+        <v>15000</v>
       </c>
       <c r="J49" s="3">
         <v>0</v>
@@ -2484,31 +2511,31 @@
         <v>60</v>
       </c>
       <c r="B50" s="2">
-        <v>322</v>
+        <v>277</v>
       </c>
       <c r="C50" s="2">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="D50" s="2">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
       </c>
       <c r="F50" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G50" s="2">
-        <v>322</v>
+        <v>247</v>
       </c>
       <c r="H50" s="2">
-        <v>322</v>
+        <v>247</v>
       </c>
       <c r="I50" s="2">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="J50" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K50" s="3">
         <v>0</v>
@@ -2522,7 +2549,7 @@
         <v>61</v>
       </c>
       <c r="B51" s="2">
-        <v>4150</v>
+        <v>29</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
@@ -2537,13 +2564,13 @@
         <v>0</v>
       </c>
       <c r="G51" s="2">
-        <v>4150</v>
+        <v>29</v>
       </c>
       <c r="H51" s="2">
-        <v>4150</v>
+        <v>29</v>
       </c>
       <c r="I51" s="2">
-        <v>5000</v>
+        <v>50</v>
       </c>
       <c r="J51" s="3">
         <v>0</v>
@@ -2560,13 +2587,13 @@
         <v>62</v>
       </c>
       <c r="B52" s="2">
-        <v>4500</v>
+        <v>273</v>
       </c>
       <c r="C52" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D52" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E52" s="2">
         <v>0</v>
@@ -2575,13 +2602,13 @@
         <v>0</v>
       </c>
       <c r="G52" s="2">
-        <v>4500</v>
+        <v>249</v>
       </c>
       <c r="H52" s="2">
-        <v>4500</v>
+        <v>249</v>
       </c>
       <c r="I52" s="2">
-        <v>5000</v>
+        <v>250</v>
       </c>
       <c r="J52" s="3">
         <v>0</v>
@@ -2598,7 +2625,7 @@
         <v>63</v>
       </c>
       <c r="B53" s="2">
-        <v>1372</v>
+        <v>246</v>
       </c>
       <c r="C53" s="2">
         <v>0</v>
@@ -2613,13 +2640,13 @@
         <v>0</v>
       </c>
       <c r="G53" s="2">
-        <v>1372</v>
+        <v>246</v>
       </c>
       <c r="H53" s="2">
-        <v>1372</v>
+        <v>246</v>
       </c>
       <c r="I53" s="2">
-        <v>1500</v>
+        <v>250</v>
       </c>
       <c r="J53" s="3">
         <v>0</v>
@@ -2636,7 +2663,7 @@
         <v>64</v>
       </c>
       <c r="B54" s="2">
-        <v>700</v>
+        <v>322</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
@@ -2651,13 +2678,13 @@
         <v>0</v>
       </c>
       <c r="G54" s="2">
-        <v>700</v>
+        <v>322</v>
       </c>
       <c r="H54" s="2">
-        <v>700</v>
+        <v>322</v>
       </c>
       <c r="I54" s="2">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="J54" s="3">
         <v>0</v>
@@ -2674,13 +2701,13 @@
         <v>65</v>
       </c>
       <c r="B55" s="2">
-        <v>3578</v>
+        <v>4150</v>
       </c>
       <c r="C55" s="2">
-        <v>2171</v>
+        <v>0</v>
       </c>
       <c r="D55" s="2">
-        <v>2171</v>
+        <v>0</v>
       </c>
       <c r="E55" s="2">
         <v>0</v>
@@ -2689,10 +2716,10 @@
         <v>0</v>
       </c>
       <c r="G55" s="2">
-        <v>1407</v>
+        <v>4150</v>
       </c>
       <c r="H55" s="2">
-        <v>1407</v>
+        <v>4150</v>
       </c>
       <c r="I55" s="2">
         <v>5000</v>
@@ -2712,7 +2739,7 @@
         <v>66</v>
       </c>
       <c r="B56" s="2">
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
@@ -2727,13 +2754,13 @@
         <v>0</v>
       </c>
       <c r="G56" s="2">
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="H56" s="2">
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="I56" s="2">
-        <v>30</v>
+        <v>5000</v>
       </c>
       <c r="J56" s="3">
         <v>0</v>
@@ -2750,7 +2777,7 @@
         <v>67</v>
       </c>
       <c r="B57" s="2">
-        <v>14</v>
+        <v>1372</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -2765,13 +2792,13 @@
         <v>0</v>
       </c>
       <c r="G57" s="2">
-        <v>14</v>
+        <v>1372</v>
       </c>
       <c r="H57" s="2">
-        <v>14</v>
+        <v>1372</v>
       </c>
       <c r="I57" s="2">
-        <v>30</v>
+        <v>1500</v>
       </c>
       <c r="J57" s="3">
         <v>0</v>
@@ -2788,36 +2815,378 @@
         <v>68</v>
       </c>
       <c r="B58" s="2">
+        <v>700</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2">
+        <v>700</v>
+      </c>
+      <c r="H58" s="2">
+        <v>700</v>
+      </c>
+      <c r="I58" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J58" s="3">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3">
+        <v>0</v>
+      </c>
+      <c r="L58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="2">
+        <v>3578</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2171</v>
+      </c>
+      <c r="D59" s="2">
+        <v>2171</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1407</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1407</v>
+      </c>
+      <c r="I59" s="2">
+        <v>5000</v>
+      </c>
+      <c r="J59" s="3">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2">
+        <v>30</v>
+      </c>
+      <c r="J60" s="3">
+        <v>0</v>
+      </c>
+      <c r="K60" s="3">
+        <v>0</v>
+      </c>
+      <c r="L60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" s="2">
+        <v>14</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0</v>
+      </c>
+      <c r="G61" s="2">
+        <v>14</v>
+      </c>
+      <c r="H61" s="2">
+        <v>14</v>
+      </c>
+      <c r="I61" s="2">
+        <v>30</v>
+      </c>
+      <c r="J61" s="3">
+        <v>0</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0</v>
+      </c>
+      <c r="L61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" s="2">
         <v>23</v>
       </c>
-      <c r="C58" s="2">
-        <v>0</v>
-      </c>
-      <c r="D58" s="2">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2">
-        <v>0</v>
-      </c>
-      <c r="G58" s="2">
+      <c r="C62" s="2">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2">
         <v>23</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H62" s="2">
         <v>23</v>
       </c>
-      <c r="I58" s="2">
+      <c r="I62" s="2">
         <v>36</v>
       </c>
-      <c r="J58" s="3">
-        <v>0</v>
-      </c>
-      <c r="K58" s="3">
-        <v>0</v>
-      </c>
-      <c r="L58" s="3">
+      <c r="J62" s="3">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0</v>
+      </c>
+      <c r="L62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <v>100</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0</v>
+      </c>
+      <c r="K63" s="3">
+        <v>0</v>
+      </c>
+      <c r="L63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0</v>
+      </c>
+      <c r="I64" s="2">
+        <v>375</v>
+      </c>
+      <c r="J64" s="3">
+        <v>0</v>
+      </c>
+      <c r="K64" s="3">
+        <v>0</v>
+      </c>
+      <c r="L64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0</v>
+      </c>
+      <c r="I65" s="2">
+        <v>340</v>
+      </c>
+      <c r="J65" s="3">
+        <v>0</v>
+      </c>
+      <c r="K65" s="3">
+        <v>0</v>
+      </c>
+      <c r="L65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0</v>
+      </c>
+      <c r="I66" s="2">
+        <v>360</v>
+      </c>
+      <c r="J66" s="3">
+        <v>0</v>
+      </c>
+      <c r="K66" s="3">
+        <v>0</v>
+      </c>
+      <c r="L66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2">
+        <v>0</v>
+      </c>
+      <c r="G67" s="2">
+        <v>0</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0</v>
+      </c>
+      <c r="I67" s="2">
+        <v>320</v>
+      </c>
+      <c r="J67" s="3">
+        <v>0</v>
+      </c>
+      <c r="K67" s="3">
+        <v>0</v>
+      </c>
+      <c r="L67" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>